<commit_message>
[fix] updated the plots for pdp example
</commit_message>
<xml_diff>
--- a/data.summary.completed.xlsx
+++ b/data.summary.completed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="509">
   <si>
     <t>data.id</t>
   </si>
@@ -1570,6 +1570,9 @@
   </si>
   <si>
     <t>Livestock, pasture / Meteo / Geography / pollution / astronomy / Geology</t>
+  </si>
+  <si>
+    <t>BNG</t>
   </si>
 </sst>
 </file>
@@ -1999,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="I284" sqref="I284"/>
+    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="K302" sqref="K302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2993,7 +2996,7 @@
         <v>4</v>
       </c>
       <c r="F36" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" s="5">
         <v>1</v>
@@ -3019,7 +3022,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" s="5">
         <v>0</v>
@@ -3825,7 +3828,7 @@
         <v>8</v>
       </c>
       <c r="F68" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" s="5">
         <v>1</v>
@@ -5735,7 +5738,7 @@
         <v>8</v>
       </c>
       <c r="F144" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G144" s="5">
         <v>1</v>
@@ -5761,7 +5764,7 @@
         <v>8</v>
       </c>
       <c r="F145" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G145" s="5">
         <v>1</v>
@@ -6367,7 +6370,7 @@
         <v>4</v>
       </c>
       <c r="F169" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G169" s="5">
         <v>1</v>
@@ -7477,7 +7480,7 @@
         <v>0</v>
       </c>
       <c r="G214" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I214" s="5" t="s">
         <v>474</v>
@@ -7875,26 +7878,26 @@
         <v>480</v>
       </c>
     </row>
-    <row r="231" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A231" s="6">
+    <row r="231" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A231" s="5">
         <v>8910</v>
       </c>
-      <c r="B231" s="6">
+      <c r="B231" s="5">
         <v>847</v>
       </c>
-      <c r="C231" s="6" t="s">
+      <c r="C231" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="D231" s="6">
+      <c r="D231" s="5">
         <v>6574</v>
       </c>
-      <c r="E231" s="6">
+      <c r="E231" s="5">
         <v>15</v>
       </c>
-      <c r="F231" s="6">
-        <v>1</v>
-      </c>
-      <c r="G231" s="6">
+      <c r="F231" s="5">
+        <v>0</v>
+      </c>
+      <c r="G231" s="5">
         <v>0</v>
       </c>
     </row>
@@ -7996,7 +7999,7 @@
         <v>0</v>
       </c>
       <c r="G235" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I235" s="5" t="s">
         <v>484</v>
@@ -8639,50 +8642,56 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A262" s="2">
+    <row r="262" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A262" s="9">
         <v>554</v>
       </c>
-      <c r="B262" s="2">
+      <c r="B262" s="9">
         <v>137</v>
       </c>
-      <c r="C262" s="2" t="s">
+      <c r="C262" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="D262" s="2">
+      <c r="D262" s="9">
         <v>39366</v>
       </c>
-      <c r="E262" s="2">
+      <c r="E262" s="9">
         <v>10</v>
       </c>
-      <c r="F262" s="2">
-        <v>0</v>
-      </c>
-      <c r="G262" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A263" s="8">
+      <c r="F262" s="9">
+        <v>0</v>
+      </c>
+      <c r="G262" s="9">
+        <v>0</v>
+      </c>
+      <c r="I262" s="9" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A263" s="9">
         <v>1042</v>
       </c>
-      <c r="B263" s="8">
+      <c r="B263" s="9">
         <v>251</v>
       </c>
-      <c r="C263" s="8" t="s">
+      <c r="C263" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="D263" s="8">
+      <c r="D263" s="9">
         <v>39366</v>
       </c>
-      <c r="E263" s="8">
+      <c r="E263" s="9">
         <v>10</v>
       </c>
-      <c r="F263" s="8">
-        <v>1</v>
-      </c>
-      <c r="G263" s="8">
-        <v>0</v>
+      <c r="F263" s="9">
+        <v>0</v>
+      </c>
+      <c r="G263" s="9">
+        <v>0</v>
+      </c>
+      <c r="I263" s="9" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.2">
@@ -8878,7 +8887,7 @@
         <v>0</v>
       </c>
       <c r="G271" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I271" s="5" t="s">
         <v>495</v>
@@ -9962,6 +9971,9 @@
       <c r="G314" s="9">
         <v>0</v>
       </c>
+      <c r="I314" s="9" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="315" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A315" s="9">
@@ -9985,6 +9997,9 @@
       <c r="G315" s="9">
         <v>0</v>
       </c>
+      <c r="I315" s="9" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="316" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A316" s="9">
@@ -10008,6 +10023,9 @@
       <c r="G316" s="9">
         <v>0</v>
       </c>
+      <c r="I316" s="9" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="317" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A317" s="9">
@@ -10031,6 +10049,9 @@
       <c r="G317" s="9">
         <v>0</v>
       </c>
+      <c r="I317" s="9" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="318" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A318" s="9">
@@ -10054,6 +10075,9 @@
       <c r="G318" s="9">
         <v>0</v>
       </c>
+      <c r="I318" s="9" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="319" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A319" s="9">
@@ -10077,6 +10101,9 @@
       <c r="G319" s="9">
         <v>0</v>
       </c>
+      <c r="I319" s="9" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="320" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A320" s="9">
@@ -10099,6 +10126,9 @@
       </c>
       <c r="G320" s="9">
         <v>0</v>
+      </c>
+      <c r="I320" s="9" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>